<commit_message>
Added date conversion method
</commit_message>
<xml_diff>
--- a/input_files/AUS.xlsx
+++ b/input_files/AUS.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="aus" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="ind" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Unique ID</t>
   </si>
@@ -164,11 +163,11 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.44"/>
@@ -176,7 +175,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.33"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -193,7 +192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -210,7 +209,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -227,7 +226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -252,62 +251,6 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>